<commit_message>
Added the BOM for the Tentacle Tip
</commit_message>
<xml_diff>
--- a/PCB Design/Fabrication/BOM.xlsx
+++ b/PCB Design/Fabrication/BOM.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tentacle Module" sheetId="1" r:id="rId1"/>
+    <sheet name="Tentacle Tip" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="tentacle_module_BOM" localSheetId="0">Sheet1!$A$1:$K$21</definedName>
+    <definedName name="tentacle_module_BOM" localSheetId="0">'Tentacle Module'!$A$1:$K$21</definedName>
+    <definedName name="tentacle_tip_BOM" localSheetId="1">'Tentacle Tip'!$A$1:$K$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -45,11 +47,28 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="tentacle_tip_BOM" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Tentacle Module\tentacle_tip_BOM.csv" tab="0" semicolon="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
   <si>
     <t>Qty</t>
   </si>
@@ -292,12 +311,6 @@
   </si>
   <si>
     <t>DE3852</t>
-  </si>
-  <si>
-    <t>DE3853</t>
-  </si>
-  <si>
-    <t>DE3851</t>
   </si>
   <si>
     <t>S5477-ND, S5456-ND</t>
@@ -358,13 +371,66 @@
   <si>
     <t>296-21208-1-ND</t>
   </si>
+  <si>
+    <t>MA04-2</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>C2, C3</t>
+  </si>
+  <si>
+    <t>C-USC1206</t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>2.2k</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>ADXL345</t>
+  </si>
+  <si>
+    <t>ADXL345LONG</t>
+  </si>
+  <si>
+    <t>LGA14_LONG</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>DE1562</t>
+  </si>
+  <si>
+    <t>1276-5070-1-ND</t>
+  </si>
+  <si>
+    <t>ADXL345BCCZ-RLCT-ND</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -404,10 +470,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,6 +543,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_module_BOM" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_tip_BOM" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -743,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,29 +831,29 @@
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>77</v>
       </c>
     </row>
@@ -823,7 +894,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -843,10 +914,10 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,7 +937,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
         <v>80</v>
@@ -889,10 +960,10 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -955,7 +1026,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -978,7 +1049,7 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1001,7 +1072,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1024,7 +1095,7 @@
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1047,7 +1118,7 @@
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1070,7 +1141,7 @@
         <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1093,7 +1164,7 @@
         <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1116,7 +1187,7 @@
         <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1139,7 +1210,7 @@
         <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,7 +1253,7 @@
         <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,7 +1276,7 @@
         <v>72</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1228,7 +1299,7 @@
         <v>75</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1236,4 +1307,186 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" activeCellId="1" sqref="G7 H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added protocell module component to BOM
</commit_message>
<xml_diff>
--- a/PCB Design/Fabrication/BOM.xlsx
+++ b/PCB Design/Fabrication/BOM.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tentacle Module" sheetId="1" r:id="rId1"/>
     <sheet name="Tentacle Tip" sheetId="2" r:id="rId2"/>
+    <sheet name="Protocell Module" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="Protocell_module_BOM" localSheetId="2">'Protocell Module'!$A$1:$K$17</definedName>
     <definedName name="tentacle_module_BOM" localSheetId="0">'Tentacle Module'!$A$1:$K$21</definedName>
     <definedName name="tentacle_tip_BOM" localSheetId="1">'Tentacle Tip'!$A$1:$K$7</definedName>
   </definedNames>
@@ -30,8 +32,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tentacle_module_BOM" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr fileType="dos" sourceFile="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Tentacle Module\tentacle_module_BOM.csv" tab="0" semicolon="1">
+  <connection id="1" name="Protocell_module_BOM" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Protocell Module\Protocell_module_BOM.csv" tab="0" semicolon="1">
       <textFields count="11">
         <textField/>
         <textField/>
@@ -47,7 +49,24 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="tentacle_tip_BOM" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" name="tentacle_module_BOM" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr fileType="dos" sourceFile="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Tentacle Module\tentacle_module_BOM.csv" tab="0" semicolon="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="tentacle_tip_BOM" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Tentacle Module\tentacle_tip_BOM.csv" tab="0" semicolon="1">
       <textFields count="11">
         <textField/>
@@ -68,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="132">
   <si>
     <t>Qty</t>
   </si>
@@ -416,12 +435,72 @@
   <si>
     <t>ADXL345BCCZ-RLCT-ND</t>
   </si>
+  <si>
+    <t>558872-1</t>
+  </si>
+  <si>
+    <t>X8</t>
+  </si>
+  <si>
+    <t>AMP connector</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>X4, X5</t>
+  </si>
+  <si>
+    <t>X2, X7</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>SQP500JB-5R6</t>
+  </si>
+  <si>
+    <t>YAGEO_SQP500JB</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>AE10381-ND, AE10393-ND</t>
+  </si>
+  <si>
+    <t>NTD5867NLT4GOSCT-ND</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>490-3897-1-ND</t>
+  </si>
+  <si>
+    <t>5.6W-5-ND</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +528,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -467,16 +560,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,11 +638,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_module_BOM" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_module_BOM" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_tip_BOM" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_tip_BOM" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Protocell_module_BOM" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -815,7 +915,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" activeCellId="1" sqref="G7 H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,4 +1589,403 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>470</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>5.6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the 10uF capacitor for the ADXL345 to 1206 package
</commit_message>
<xml_diff>
--- a/PCB Design/Fabrication/BOM.xlsx
+++ b/PCB Design/Fabrication/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tentacle Module" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="133">
   <si>
     <t>Qty</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>5.6W-5-ND</t>
+  </si>
+  <si>
+    <t>1276-1075-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1413,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1543,7 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1588,6 +1591,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1595,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed 10uF caps package to 1206
</commit_message>
<xml_diff>
--- a/PCB Design/Fabrication/BOM.xlsx
+++ b/PCB Design/Fabrication/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Tentacle Module" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="132">
   <si>
     <t>Qty</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>1276-1012-1-ND</t>
-  </si>
-  <si>
-    <t>490-7198-1-ND</t>
   </si>
   <si>
     <r>
@@ -917,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,10 +1137,10 @@
         <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -1152,7 +1149,7 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1175,7 +1172,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1198,7 +1195,7 @@
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1221,7 +1218,7 @@
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,7 +1241,7 @@
         <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1267,7 +1264,7 @@
         <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1290,7 +1287,7 @@
         <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1313,7 +1310,7 @@
         <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,7 +1353,7 @@
         <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,7 +1376,7 @@
         <v>72</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,7 +1399,7 @@
         <v>75</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1416,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -1477,7 +1474,7 @@
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1491,7 +1488,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -1505,7 +1502,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1514,7 +1511,7 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
@@ -1531,10 +1528,10 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" t="s">
-        <v>102</v>
       </c>
       <c r="E5" t="s">
         <v>50</v>
@@ -1543,7 +1540,7 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1551,7 +1548,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
@@ -1560,13 +1557,13 @@
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1574,19 +1571,19 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
         <v>105</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>106</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>107</v>
       </c>
-      <c r="E7" t="s">
-        <v>108</v>
-      </c>
       <c r="G7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1647,19 +1644,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
         <v>112</v>
       </c>
-      <c r="D2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>113</v>
       </c>
-      <c r="F2" t="s">
-        <v>114</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,7 +1670,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -1693,7 +1690,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -1713,13 +1710,13 @@
         <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
         <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1733,7 +1730,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -1756,7 +1753,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -1773,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
@@ -1782,13 +1779,13 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1822,7 +1819,7 @@
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F10" t="s">
         <v>30</v>
@@ -1836,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -1845,13 +1842,13 @@
         <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
         <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1874,7 +1871,7 @@
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1897,7 +1894,7 @@
         <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1908,16 +1905,16 @@
         <v>5.6</v>
       </c>
       <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" t="s">
         <v>123</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>124</v>
       </c>
-      <c r="E14" t="s">
-        <v>125</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1940,7 +1937,7 @@
         <v>55</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1957,13 +1954,13 @@
         <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" t="s">
         <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1986,7 +1983,7 @@
         <v>72</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>